<commit_message>
Mudança no código "Automação em excel"
A principal diferença entre os dois códigos é que o primeiro código trabalha com um arquivo Excel existente, enquanto o segundo código cria um novo arquivo. Além disso, o segundo código converte a cor para o formato RGB, enquanto o primeiro código não.
</commit_message>
<xml_diff>
--- a/relatorio_excel.xlsx
+++ b/relatorio_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Desktop\Programação\Scripts python\Meus projetos em python\Importando-bibliotecas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C7ADD32-65CE-4F8C-A016-32DA1E178E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{227A4722-E760-4391-9B1A-4E23B6A51E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6255" yWindow="2370" windowWidth="21600" windowHeight="11835" xr2:uid="{78589423-B470-4441-B310-7EF9C1998440}"/>
+    <workbookView xWindow="6255" yWindow="2370" windowWidth="21600" windowHeight="11835" xr2:uid="{7360DAA3-5B56-4705-BE23-119DF84B36B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5CF52D-91D4-4689-A63D-DCDF3915149F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595DE73F-5F6E-476F-B518-10C89D9CE906}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>